<commit_message>
changed url to localhost for development, removed extra lines in xlsx
</commit_message>
<xml_diff>
--- a/CurrentWeekAccounts.xlsx
+++ b/CurrentWeekAccounts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cs_projects\SCBC_SS2020\SCBC_SnackShackServer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cs_projects\SCBC_SnackShack\SCBC_SnackShackServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D7CE2E-6A06-4EDD-A461-C25FC99B8443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE526E5-5685-4BF8-83ED-4A7C9CB72484}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1910,20 +1910,6 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B68">
-        <f>SUM(B2:B67)</f>
-        <v>1535</v>
-      </c>
-      <c r="C68">
-        <f>SUM(C2:C67)</f>
-        <v>1298.25</v>
-      </c>
-      <c r="D68">
-        <f>SUM(D2:D66)</f>
-        <v>236.75</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>